<commit_message>
Added the Single MG with heat, Electnet and Evs
</commit_message>
<xml_diff>
--- a/Results/SingleMG_ElectAndHeatNet.xlsx
+++ b/Results/SingleMG_ElectAndHeatNet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterWork\Codes\MicrogridOptimization\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F881C69E-EA6C-4C21-AF7D-5F20F1231E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D5E124E1-C484-465A-80FB-D866114AE481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
@@ -1039,13 +1039,13 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.57894599999999996</v>
+        <v>-0.57894599999999996</v>
       </c>
       <c r="L2">
         <v>0.39200000000000002</v>
       </c>
       <c r="M2">
-        <v>40.421100000000003</v>
+        <v>-40.421100000000003</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="W2">
-        <v>20</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -1116,7 +1116,7 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="M3">
-        <v>28</v>
+        <v>-28</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>25</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
@@ -1187,7 +1187,7 @@
         <v>0.67225000000000001</v>
       </c>
       <c r="M4">
-        <v>31</v>
+        <v>-31</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1217,7 +1217,7 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>30</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
@@ -1258,7 +1258,7 @@
         <v>0.85750000000000004</v>
       </c>
       <c r="M5">
-        <v>39</v>
+        <v>-39</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <v>30</v>
+        <v>-30</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
@@ -1329,7 +1329,7 @@
         <v>0.99524999999999997</v>
       </c>
       <c r="M6">
-        <v>29</v>
+        <v>-29</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1359,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>25</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
@@ -1400,7 +1400,7 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1430,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>15</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
@@ -1465,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>60</v>
+        <v>-60</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -1501,7 +1501,7 @@
         <v>0</v>
       </c>
       <c r="W8">
-        <v>25</v>
+        <v>-25</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.35">
@@ -1536,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>86</v>
+        <v>-86</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="W9">
-        <v>15</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.35">
@@ -1607,7 +1607,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>87</v>
+        <v>-87</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1643,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>80</v>
+        <v>-80</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.35">
@@ -1678,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>89</v>
+        <v>-89</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="W11">
-        <v>65</v>
+        <v>-65</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.35">
@@ -1749,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>183</v>
+        <v>-183</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
       <c r="W12">
-        <v>60</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.35">
@@ -1820,7 +1820,7 @@
         <v>0</v>
       </c>
       <c r="K13">
-        <v>328</v>
+        <v>-328</v>
       </c>
       <c r="L13">
         <v>0.47368399999999999</v>
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="W13">
-        <v>55</v>
+        <v>-55</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.35">
@@ -1891,7 +1891,7 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>325</v>
+        <v>-325</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1927,7 +1927,7 @@
         <v>0</v>
       </c>
       <c r="W14">
-        <v>60</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.35">
@@ -1962,7 +1962,7 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>238</v>
+        <v>-238</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="W15">
-        <v>60</v>
+        <v>-60</v>
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.35">
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>148</v>
+        <v>-148</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2069,7 +2069,7 @@
         <v>0</v>
       </c>
       <c r="W16">
-        <v>75</v>
+        <v>-75</v>
       </c>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.35">
@@ -2104,7 +2104,7 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>132</v>
+        <v>-132</v>
       </c>
       <c r="L17">
         <v>0</v>
@@ -2140,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="W17">
-        <v>85</v>
+        <v>-85</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.35">
@@ -2175,7 +2175,7 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>119</v>
+        <v>-119</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -2211,7 +2211,7 @@
         <v>0</v>
       </c>
       <c r="W18">
-        <v>70</v>
+        <v>-70</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.35">
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>79</v>
+        <v>-79</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="W19">
-        <v>65</v>
+        <v>-65</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.35">
@@ -2317,7 +2317,7 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>46</v>
+        <v>-46</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2388,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <v>163</v>
+        <v>-163</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2459,7 +2459,7 @@
         <v>0</v>
       </c>
       <c r="K22">
-        <v>202</v>
+        <v>-202</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2530,7 +2530,7 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>196</v>
+        <v>-196</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2601,7 +2601,7 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>186</v>
+        <v>-186</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2672,7 +2672,7 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>180</v>
+        <v>-180</v>
       </c>
       <c r="L25">
         <v>0</v>

</xml_diff>

<commit_message>
changed the input data
</commit_message>
<xml_diff>
--- a/Results/SingleMG_ElectAndHeatNet.xlsx
+++ b/Results/SingleMG_ElectAndHeatNet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MasterWork\Codes\MicrogridOptimization\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D5E124E1-C484-465A-80FB-D866114AE481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCA77E1D-58B7-4C0B-8330-9B03F3491D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
   </bookViews>
@@ -1036,28 +1036,28 @@
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="K2">
-        <v>-0.57894599999999996</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0.39200000000000002</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="M2">
-        <v>-40.421100000000003</v>
+        <v>-100</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
       <c r="Q2">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="R2">
         <v>100</v>
@@ -1066,7 +1066,7 @@
         <v>0</v>
       </c>
       <c r="T2">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="U2">
         <v>125</v>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="W2">
-        <v>-20</v>
+        <v>-45</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.35">
@@ -1107,28 +1107,28 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>0.52500000000000002</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="M3">
-        <v>-28</v>
+        <v>0</v>
       </c>
       <c r="N3">
         <v>0</v>
       </c>
       <c r="O3">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="R3">
         <v>100</v>
@@ -1137,7 +1137,7 @@
         <v>0</v>
       </c>
       <c r="T3">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="U3">
         <v>125</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="W3">
-        <v>-25</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.35">
@@ -1178,28 +1178,28 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>87.421099999999996</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0.67225000000000001</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>-31</v>
+        <v>-68.421099999999996</v>
       </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="R4">
         <v>100</v>
@@ -1208,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="T4">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="U4">
         <v>125</v>
@@ -1217,7 +1217,7 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <v>-30</v>
+        <v>-55</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.35">
@@ -1249,28 +1249,28 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0.85750000000000004</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>-39</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
       <c r="O5">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="R5">
         <v>100</v>
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="U5">
         <v>125</v>
@@ -1288,7 +1288,7 @@
         <v>0</v>
       </c>
       <c r="W5">
-        <v>-30</v>
+        <v>-55</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.35">
@@ -1320,28 +1320,28 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0.99524999999999997</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>-29</v>
+        <v>0</v>
       </c>
       <c r="N6">
         <v>0</v>
       </c>
       <c r="O6">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="R6">
         <v>100</v>
@@ -1350,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="T6">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="U6">
         <v>125</v>
@@ -1359,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="W6">
-        <v>-25</v>
+        <v>-50</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.35">
@@ -1367,7 +1367,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="C7">
         <v>135</v>
@@ -1391,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1400,19 +1400,19 @@
         <v>1</v>
       </c>
       <c r="M7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="R7">
         <v>100</v>
@@ -1421,7 +1421,7 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="U7">
         <v>125</v>
@@ -1430,7 +1430,7 @@
         <v>0</v>
       </c>
       <c r="W7">
-        <v>-15</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.35">
@@ -1462,10 +1462,10 @@
         <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="K8">
-        <v>-60</v>
+        <v>0</v>
       </c>
       <c r="L8">
         <v>1</v>
@@ -1477,10 +1477,10 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P8">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <v>60</v>
@@ -1533,10 +1533,10 @@
         <v>10</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="K9">
-        <v>-86</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1548,10 +1548,10 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q9">
         <v>60</v>
@@ -1604,10 +1604,10 @@
         <v>15</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="K10">
-        <v>-87</v>
+        <v>0</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1619,10 +1619,10 @@
         <v>0</v>
       </c>
       <c r="O10">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P10">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <v>60</v>
@@ -1675,10 +1675,10 @@
         <v>20</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="K11">
-        <v>-89</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1690,10 +1690,10 @@
         <v>0</v>
       </c>
       <c r="O11">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P11">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q11">
         <v>60</v>
@@ -1722,7 +1722,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>193</v>
+        <v>300</v>
       </c>
       <c r="C12">
         <v>195</v>
@@ -1746,10 +1746,10 @@
         <v>23</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="K12">
-        <v>-183</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1761,10 +1761,10 @@
         <v>0</v>
       </c>
       <c r="O12">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P12">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>60</v>
@@ -1793,7 +1793,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>158</v>
+        <v>320</v>
       </c>
       <c r="C13">
         <v>200</v>
@@ -1817,25 +1817,25 @@
         <v>28</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="K13">
-        <v>-328</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>0.47368399999999999</v>
+        <v>0.55789500000000003</v>
       </c>
       <c r="M13">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="O13">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P13">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q13">
         <v>60</v>
@@ -1864,7 +1864,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>161</v>
+        <v>280</v>
       </c>
       <c r="C14">
         <v>195</v>
@@ -1891,22 +1891,22 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>-325</v>
+        <v>0</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>0.27368399999999998</v>
       </c>
       <c r="M14">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="O14">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q14">
         <v>60</v>
@@ -1935,7 +1935,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>162</v>
+        <v>260</v>
       </c>
       <c r="C15">
         <v>195</v>
@@ -1962,22 +1962,22 @@
         <v>0</v>
       </c>
       <c r="K15">
-        <v>-238</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>0.115789</v>
       </c>
       <c r="M15">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="O15">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P15">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q15">
         <v>60</v>
@@ -2033,7 +2033,7 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>-148</v>
+        <v>0</v>
       </c>
       <c r="L16">
         <v>0</v>
@@ -2042,13 +2042,13 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="O16">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P16">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q16">
         <v>60</v>
@@ -2077,7 +2077,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="C17">
         <v>170</v>
@@ -2104,22 +2104,22 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>-132</v>
+        <v>-10.919700000000001</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>5.2631600000000001E-2</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>-11.080299999999999</v>
       </c>
       <c r="N17">
         <v>0</v>
       </c>
       <c r="O17">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <v>60</v>
@@ -2148,7 +2148,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>267</v>
+        <v>180</v>
       </c>
       <c r="C18">
         <v>185</v>
@@ -2175,10 +2175,10 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>-119</v>
+        <v>-36</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>5.2631600000000001E-2</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -2187,10 +2187,10 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P18">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q18">
         <v>60</v>
@@ -2219,7 +2219,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>271</v>
+        <v>190</v>
       </c>
       <c r="C19">
         <v>190</v>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="K19">
-        <v>-79</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <v>0</v>
@@ -2255,13 +2255,13 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O19">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P19">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q19">
         <v>60</v>
@@ -2290,7 +2290,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>284</v>
+        <v>240</v>
       </c>
       <c r="C20">
         <v>195</v>
@@ -2314,10 +2314,10 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="K20">
-        <v>-46</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2329,10 +2329,10 @@
         <v>0</v>
       </c>
       <c r="O20">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P20">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q20">
         <v>60</v>
@@ -2361,7 +2361,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>167</v>
+        <v>280</v>
       </c>
       <c r="C21">
         <v>200</v>
@@ -2385,10 +2385,10 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="K21">
-        <v>-163</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2400,10 +2400,10 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P21">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q21">
         <v>60</v>
@@ -2432,7 +2432,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>128</v>
+        <v>325</v>
       </c>
       <c r="C22">
         <v>195</v>
@@ -2456,10 +2456,10 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>165</v>
       </c>
       <c r="K22">
-        <v>-202</v>
+        <v>0</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2471,10 +2471,10 @@
         <v>0</v>
       </c>
       <c r="O22">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P22">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q22">
         <v>60</v>
@@ -2503,7 +2503,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>134</v>
+        <v>350</v>
       </c>
       <c r="C23">
         <v>190</v>
@@ -2527,10 +2527,10 @@
         <v>0</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>190</v>
       </c>
       <c r="K23">
-        <v>-196</v>
+        <v>0</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -2542,10 +2542,10 @@
         <v>0</v>
       </c>
       <c r="O23">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P23">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q23">
         <v>60</v>
@@ -2574,7 +2574,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>144</v>
+        <v>300</v>
       </c>
       <c r="C24">
         <v>180</v>
@@ -2598,10 +2598,10 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="K24">
-        <v>-186</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -2613,10 +2613,10 @@
         <v>0</v>
       </c>
       <c r="O24">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P24">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q24">
         <v>60</v>
@@ -2645,7 +2645,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>150</v>
+        <v>250</v>
       </c>
       <c r="C25">
         <v>175</v>
@@ -2669,10 +2669,10 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="K25">
-        <v>-180</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2684,10 +2684,10 @@
         <v>0</v>
       </c>
       <c r="O25">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="P25">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="Q25">
         <v>60</v>

</xml_diff>